<commit_message>
feat: atualizar planilhas modelo de calendário, eventos, horários e provas
</commit_message>
<xml_diff>
--- a/templates/planilha_modelo_calendario.xlsx
+++ b/templates/planilha_modelo_calendario.xlsx
@@ -1,14 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29518"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70BBF8D2-34F7-4C33-A5E8-C22AC8624F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{14791E4C-E87D-4EB6-A6FA-E31024D6E4C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Calendario" sheetId="1" r:id="rId1"/>
+    <sheet name="Lista periodos" sheetId="2" r:id="rId2"/>
+    <sheet name="Lista cursos" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>titulo</t>
   </si>
@@ -52,6 +54,99 @@
   </si>
   <si>
     <t>nome_curso</t>
+  </si>
+  <si>
+    <t>1° período</t>
+  </si>
+  <si>
+    <t>2° período</t>
+  </si>
+  <si>
+    <t>3° período</t>
+  </si>
+  <si>
+    <t>4° período</t>
+  </si>
+  <si>
+    <t>5° período</t>
+  </si>
+  <si>
+    <t>6° período</t>
+  </si>
+  <si>
+    <t>7° período</t>
+  </si>
+  <si>
+    <t>8° período</t>
+  </si>
+  <si>
+    <t>Administração</t>
+  </si>
+  <si>
+    <t>Agronomia</t>
+  </si>
+  <si>
+    <t>Arquitetura e Urbanismo</t>
+  </si>
+  <si>
+    <t>Biomedicina</t>
+  </si>
+  <si>
+    <t>Ciências Biológicas</t>
+  </si>
+  <si>
+    <t>Ciências Contábeis</t>
+  </si>
+  <si>
+    <t>Comunicação Social: Publicidade e Propaganda</t>
+  </si>
+  <si>
+    <t>Design Gráfico</t>
+  </si>
+  <si>
+    <t>Direito</t>
+  </si>
+  <si>
+    <t>Educação Física</t>
+  </si>
+  <si>
+    <t>Enfermagem</t>
+  </si>
+  <si>
+    <t>Engenharia Civil</t>
+  </si>
+  <si>
+    <t>Engenharia de Software</t>
+  </si>
+  <si>
+    <t>Engenharia Elétrica</t>
+  </si>
+  <si>
+    <t>Engenharia Mecânica</t>
+  </si>
+  <si>
+    <t>Estética e Cosmética</t>
+  </si>
+  <si>
+    <t>Farmácia</t>
+  </si>
+  <si>
+    <t>Fisioterapia</t>
+  </si>
+  <si>
+    <t>Gastronomia</t>
+  </si>
+  <si>
+    <t>Gestão Pública</t>
+  </si>
+  <si>
+    <t>Psicologia</t>
+  </si>
+  <si>
+    <t>Medicina</t>
+  </si>
+  <si>
+    <t>Relações Internacionais</t>
   </si>
 </sst>
 </file>
@@ -95,14 +190,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -113,6 +217,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6AAA2C7A-E141-488C-B1EB-DE4017E5F73C}" name="Tabela1" displayName="Tabela1" ref="A1:G2" totalsRowShown="0">
+  <autoFilter ref="A1:G2" xr:uid="{6AAA2C7A-E141-488C-B1EB-DE4017E5F73C}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{55F22B5D-AF92-464E-96E1-E12B38061984}" name="titulo"/>
+    <tableColumn id="2" xr3:uid="{78AC3C8D-FE9E-4DD7-BB0C-3B787F1C57BF}" name="data" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{F6F283C8-9C8D-45B5-8C19-91A072EA8833}" name="tipo"/>
+    <tableColumn id="4" xr3:uid="{14A9054C-DCC7-4056-9823-7AF39971960C}" name="descricao"/>
+    <tableColumn id="5" xr3:uid="{B89B085B-EC9B-4FF0-A3C5-C871BFC711FB}" name="semestre"/>
+    <tableColumn id="6" xr3:uid="{80B20C48-AFEE-405C-883D-E7805F7C433F}" name="ano" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{53479351-825C-4604-960A-CB5EF7001BB7}" name="nome_curso"/>
+  </tableColumns>
+  <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,20 +522,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="3"/>
+    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -427,7 +551,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -439,5 +563,213 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C400D92F-CBD8-446A-9493-A44B3DC56FF2}">
+          <x14:formula1>
+            <xm:f>'Lista periodos'!$A$1:$A$8</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F6A3B37A-D32D-4512-BE66-EBDBE34CEAAE}">
+          <x14:formula1>
+            <xm:f>'Lista cursos'!$A$1:$A$23</xm:f>
+          </x14:formula1>
+          <xm:sqref>G1:G1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0687928-C043-40D6-B8B8-6293DFE08E7D}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F8AA77-FC0D-4855-8F1E-6C08B4FF477E}">
+  <dimension ref="A1:A23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="41.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1">
+      <c r="A18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1">
+      <c r="A20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1">
+      <c r="A21" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1">
+      <c r="A22" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1">
+      <c r="A23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>